<commit_message>
additions for v2.13 framework and updates
</commit_message>
<xml_diff>
--- a/data/Frameworks/CCIsUpload.xlsx
+++ b/data/Frameworks/CCIsUpload.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>CCI ID</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>policy, technical</t>
+  </si>
+  <si>
+    <t>HITRUST Alliance HITRUST CSF v11.5.0 Authoritative Sources Cross-Reference.xlsx</t>
   </si>
   <si>
     <t>CCI-100002</t>
@@ -368,7 +371,7 @@
     <col customWidth="1" min="4" max="4" width="23.63"/>
     <col customWidth="1" min="5" max="5" width="18.25"/>
     <col customWidth="1" min="6" max="6" width="20.38"/>
-    <col customWidth="1" min="7" max="7" width="19.13"/>
+    <col customWidth="1" min="7" max="7" width="44.88"/>
     <col customWidth="1" min="8" max="8" width="20.25"/>
   </cols>
   <sheetData>
@@ -436,7 +439,9 @@
       <c r="F2" s="4">
         <v>45829.0</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -460,10 +465,10 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -477,7 +482,9 @@
       <c r="F3" s="4">
         <v>45829.0</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -501,10 +508,10 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
@@ -518,7 +525,9 @@
       <c r="F4" s="4">
         <v>45829.0</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -542,10 +551,10 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
@@ -559,7 +568,9 @@
       <c r="F5" s="4">
         <v>45829.0</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>

</xml_diff>